<commit_message>
update response speed and retry logic
</commit_message>
<xml_diff>
--- a/tests/e2e_tests/test-workbooks/Alibaba_IPO_Financial_Model_Excel_Template_d1d057d0d2.xlsx
+++ b/tests/e2e_tests/test-workbooks/Alibaba_IPO_Financial_Model_Excel_Template_d1d057d0d2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shrey\projects\core-models-xls-model\data\exemplar\IPO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shrey\OfficeAddinApps\core-models-excel-addin\tests\e2e_tests\test-workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DEB4C2-36F0-423A-8F2C-80B1009E0831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D19D26F-3144-4194-8A8E-A9A2B8BA694D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="29020" windowHeight="15700" tabRatio="595" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="20" r:id="rId1"/>
@@ -4056,12 +4056,8 @@
   </sheetPr>
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="N27" sqref="N27"/>
-      <selection pane="topRight" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4669,12 +4665,8 @@
   </sheetPr>
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="N27" sqref="N27"/>
-      <selection pane="topRight" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="11.5"/>
@@ -5098,11 +5090,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="N27" sqref="N27"/>
-      <selection pane="topRight" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
@@ -5570,11 +5558,7 @@
   <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="N27" sqref="N27"/>
-      <selection pane="topRight" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14"/>
@@ -7293,7 +7277,7 @@
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14" outlineLevelRow="1"/>
@@ -18371,8 +18355,8 @@
   </sheetPr>
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -20478,12 +20462,8 @@
   </sheetPr>
   <dimension ref="A1:V87"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="N27" sqref="N27"/>
-      <selection pane="topRight" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -23667,12 +23647,8 @@
   </sheetPr>
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="N27" sqref="N27"/>
-      <selection pane="topRight" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
-      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -24359,12 +24335,8 @@
   </sheetPr>
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="D4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="H9" sqref="H9"/>
-      <selection pane="topRight" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>

</xml_diff>